<commit_message>
added resazurin test script
</commit_message>
<xml_diff>
--- a/data/environmental/loggers.xlsx
+++ b/data/environmental/loggers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/polyIC-larvae/data/environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F1512-F31C-D945-8F46-D15015D2F297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D18FAD8-E061-F14E-88B7-C0BBAB884993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
+    <workbookView xWindow="660" yWindow="3180" windowWidth="27240" windowHeight="16440" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>logger</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>group</t>
+  </si>
+  <si>
+    <t>FTR-left</t>
+  </si>
+  <si>
+    <t>FTR-right</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB36B54-B7B4-0742-A47F-176219A7FAF5}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,6 +487,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>